<commit_message>
Agregue palabras al arreglo de palabras, modifique estructurasDatosWordix
</commit_message>
<xml_diff>
--- a/estructurasDatosWordix.xlsx
+++ b/estructurasDatosWordix.xlsx
@@ -1,13 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25830"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB62B6BD-7F83-46B0-8C5B-B05E9AB977B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="EstructuraDatos" sheetId="1" r:id="rId4"/>
+    <sheet name="EstructuraDatos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mixDXI+aB4LTtOYfgg4FvHy9KOjvg=="/>
     </ext>
@@ -16,7 +31,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+  <si>
+    <t>GRUPO 8: Cruz Oviedo, De Phillipis, Padilla</t>
+  </si>
+  <si>
+    <t>Representacion del arreglo $coleccionPalabras</t>
+  </si>
   <si>
     <t>$coleccionPalabras=</t>
   </si>
@@ -42,13 +63,28 @@
     <t>GATOS</t>
   </si>
   <si>
+    <t>GOTAS</t>
+  </si>
+  <si>
+    <t>HUEVO</t>
+  </si>
+  <si>
+    <t>TINTO</t>
+  </si>
+  <si>
+    <t>NAVES</t>
+  </si>
+  <si>
+    <t>VERDE</t>
+  </si>
+  <si>
     <t>//valores</t>
   </si>
   <si>
     <t>Información de la estructura:</t>
   </si>
   <si>
-    <t>Tipo: Indexado (los índices son numéricos)</t>
+    <t>Tipo: Indexado</t>
   </si>
   <si>
     <t>Tipos de datos: Almacena valores String</t>
@@ -57,59 +93,124 @@
     <t>¿Para qué se utilizada?: guarda las palabras que se pueden utilizar para jugar wordix</t>
   </si>
   <si>
-    <t>**** SEGUIR COMPLETANDO ****</t>
+    <t>Representacion del arreglo $coleccionPartidas</t>
+  </si>
+  <si>
+    <t>Claves
+|
+v</t>
+  </si>
+  <si>
+    <t>$coleccionPartidas=</t>
+  </si>
+  <si>
+    <t>palabraWordix</t>
+  </si>
+  <si>
+    <t>Tipo: Asociativa</t>
+  </si>
+  <si>
+    <t>jugador</t>
+  </si>
+  <si>
+    <t>majo</t>
+  </si>
+  <si>
+    <t>rudolf</t>
+  </si>
+  <si>
+    <t>pink2000</t>
+  </si>
+  <si>
+    <t>Tipos de datos: Almacena valores String e Integer</t>
+  </si>
+  <si>
+    <t>intentos</t>
+  </si>
+  <si>
+    <t>¿Para qué es utilizada?: Guardar los datos de las partidas jugadas</t>
+  </si>
+  <si>
+    <t>puntaje</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
     </font>
     <font>
       <i/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -123,54 +224,75 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color rgb="FF000000"/>
-      </right>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -360,115 +482,290 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.86"/>
-    <col customWidth="1" min="2" max="2" width="14.29"/>
-    <col customWidth="1" min="3" max="3" width="13.43"/>
-    <col customWidth="1" min="4" max="4" width="13.71"/>
-    <col customWidth="1" min="5" max="5" width="12.86"/>
-    <col customWidth="1" min="6" max="6" width="12.29"/>
-    <col customWidth="1" min="7" max="7" width="12.0"/>
-    <col customWidth="1" min="8" max="26" width="10.71"/>
+    <col min="1" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="14" width="12" customWidth="1"/>
+    <col min="15" max="33" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="1" spans="1:15" ht="15" customHeight="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>5.0</v>
-      </c>
-      <c r="H3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:15" ht="15" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:15" ht="15" customHeight="1">
+      <c r="A4" s="7"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="H5" s="2">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="I5" s="2">
         <v>5</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="J5" s="2">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="K5" s="2">
         <v>7</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="L5" s="2">
         <v>8</v>
       </c>
+      <c r="M5" s="2">
+        <v>9</v>
+      </c>
+      <c r="N5" s="2">
+        <v>10</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:15">
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>9</v>
       </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7">
-      <c r="B7" s="1" t="s">
+    <row r="8" spans="1:15">
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" customHeight="1">
+      <c r="A13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" customHeight="1">
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2">
+        <v>3</v>
+      </c>
+      <c r="K15" s="2">
+        <v>4</v>
+      </c>
+      <c r="L15" s="2">
+        <v>5</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" customHeight="1">
+      <c r="B16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" ht="15" customHeight="1">
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" ht="15" customHeight="1">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="9">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9">
+        <v>3</v>
+      </c>
+      <c r="I18" s="9">
+        <v>6</v>
+      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" ht="15" customHeight="1">
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="9">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9">
+        <v>14</v>
+      </c>
+      <c r="I19" s="9">
         <v>10</v>
       </c>
+      <c r="J19" s="9"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="12" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="8">
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="23" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="24" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="25" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="26" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="27" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="28" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="29" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="30" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="31" spans="3:13" ht="15.75" customHeight="1"/>
+    <row r="32" spans="3:13" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1437,10 +1734,13 @@
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <mergeCells count="1">
+    <mergeCell ref="F13:F15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>